<commit_message>
menu edited and port 80
</commit_message>
<xml_diff>
--- a/functions/menus/barfood.xlsx
+++ b/functions/menus/barfood.xlsx
@@ -5,28 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\URBANFOODCOURT1\Users\FC1\OneDrive\Documents\mall-restaurant\functions\menus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ef994ddc3fa0009/Documents/mall-restaurant/functions/menus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDA2E2-DAA7-444D-81F8-FAD9D35D79DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{89EDA2E2-DAA7-444D-81F8-FAD9D35D79DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3FDFE86-D717-46D7-B119-589322880B4C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="11" xr2:uid="{913ECFC5-BE82-444D-A9C6-21D36117BB0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="14" xr2:uid="{913ECFC5-BE82-444D-A9C6-21D36117BB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="DRINKS" sheetId="1" r:id="rId1"/>
     <sheet name="JUICES" sheetId="2" r:id="rId2"/>
-    <sheet name="VEG. SOUP" sheetId="3" r:id="rId3"/>
-    <sheet name="NON. VEG. SOUP" sheetId="4" r:id="rId4"/>
+    <sheet name="VEG SOUP" sheetId="3" r:id="rId3"/>
+    <sheet name="NON VEG SOUP" sheetId="4" r:id="rId4"/>
     <sheet name="LASSI" sheetId="5" r:id="rId5"/>
-    <sheet name="SNACKS NON VEG." sheetId="6" r:id="rId6"/>
-    <sheet name="SNACKS VEG." sheetId="7" r:id="rId7"/>
-    <sheet name="TANDOORI VEG." sheetId="8" r:id="rId8"/>
-    <sheet name="INDIAN CURRIES VEG." sheetId="11" r:id="rId9"/>
+    <sheet name="SNACKS NON VEG" sheetId="6" r:id="rId6"/>
+    <sheet name="SNACKS VEG" sheetId="7" r:id="rId7"/>
+    <sheet name="TANDOORI VEG" sheetId="8" r:id="rId8"/>
+    <sheet name="INDIAN CURRIES VEG" sheetId="11" r:id="rId9"/>
     <sheet name="SALAD" sheetId="12" r:id="rId10"/>
     <sheet name="RAITA" sheetId="13" r:id="rId11"/>
-    <sheet name="TANDOOR NON VEG." sheetId="14" r:id="rId12"/>
+    <sheet name="TANDOOR NON VEG" sheetId="14" r:id="rId12"/>
     <sheet name="RICE &amp; BIRYANI" sheetId="9" r:id="rId13"/>
-    <sheet name="INDIAN CURRIES NON VEG." sheetId="10" r:id="rId14"/>
+    <sheet name="INDIAN CURRIES NON VEG" sheetId="10" r:id="rId14"/>
     <sheet name="BREAD" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <si>
     <t>WATER BOTTLE</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>JAIRY MAIRY CHICKEN</t>
+  </si>
+  <si>
+    <t>EGG Pakoda</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558AF246-61CB-44C9-86BB-43FB08F458C0}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1879,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23629338-B275-4F69-8019-C2697E75E994}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2127,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4937C7-CB77-4735-816A-DCC210C4E7E8}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,6 +2807,14 @@
       </c>
       <c r="B44" s="3">
         <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" s="3">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>